<commit_message>
updated data shared with comms
</commit_message>
<xml_diff>
--- a/shared_data/Costs for web team 2021 v2.xlsx
+++ b/shared_data/Costs for web team 2021 v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csgorg-my.sharepoint.com/personal/mroberts_csg_org/Documents/Desktop/csgjc/repos/cc_survey/shared_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mroberts\OneDrive - The Council of State Governments\Desktop\csgjc\repos\cc_survey\shared_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_D852EFF02D997DEF6CC40BB751F328C8996B57D4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{909CA3E5-920E-4C6E-82B4-C3A26663A64D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD1E811-DFD4-488F-8408-E235781FDBA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="135" windowWidth="13140" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7965" yWindow="0" windowWidth="18780" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
     <t>Average yearly cost</t>
   </si>
   <si>
-    <t>Change from 2019-2020</t>
+    <t>Cost Savings from Violation Change from 2019-2020</t>
   </si>
 </sst>
 </file>
@@ -101,9 +101,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,20 +406,20 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -429,8 +432,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
@@ -444,8 +447,8 @@
         <v>47853072544.52697</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3">
@@ -459,8 +462,8 @@
         <v>11148215042.835747</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -474,8 +477,8 @@
         <v>4657016826.5106173</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5">
@@ -489,8 +492,8 @@
         <v>41950410507.928589</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6">
@@ -504,8 +507,8 @@
         <v>9034108600.1461639</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7">
@@ -519,8 +522,8 @@
         <v>3595614186.6115403</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="1">

</xml_diff>